<commit_message>
page object in add comments and booking star
</commit_message>
<xml_diff>
--- a/tests/Assets/Comments.xlsx
+++ b/tests/Assets/Comments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">rahulj+1@qburst.com</t>
   </si>
@@ -28,10 +28,7 @@
     <t xml:space="preserve">https://starsona-dev.qburst.build/ranveersingh</t>
   </si>
   <si>
-    <t xml:space="preserve">//div[@id='video-0']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234567@</t>
+    <t xml:space="preserve">#video-0</t>
   </si>
   <si>
     <t xml:space="preserve">rahulj+56@qburst.com</t>
@@ -40,7 +37,7 @@
     <t xml:space="preserve">https://starsona-dev.qburst.build/johnnybravo</t>
   </si>
   <si>
-    <t xml:space="preserve">//div[@id='video-1']</t>
+    <t xml:space="preserve">#video-1</t>
   </si>
   <si>
     <t xml:space="preserve">rahulj+lion@qburst.com</t>
@@ -237,7 +234,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
@@ -258,55 +255,40 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>